<commit_message>
Added files from Iteration 2
</commit_message>
<xml_diff>
--- a/product/ProductVisionBoard.xlsx
+++ b/product/ProductVisionBoard.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
   <si>
     <t>Our vision is to create an application which delivers an full and completely managed fridge as a service to our user and costumers with the benefits of ecological and healthcare reliability.</t>
   </si>
@@ -28,7 +31,7 @@
     <t>Geschäftsziele</t>
   </si>
   <si>
-    <t>Familien</t>
+    <t>Haushalte</t>
   </si>
   <si>
     <t>Keine Lebensmittel wegschmeißen zu müssen</t>
@@ -40,7 +43,7 @@
     <t>Vereinfachen der Kühlschrankverwaltung</t>
   </si>
   <si>
-    <t>Kühlschrankgemeinschaften in Betrieben oder WG´s</t>
+    <t>Kühlschrankgemeinschaften</t>
   </si>
   <si>
     <t>Immer genügend zu Essen im Kühlschrank</t>
@@ -52,7 +55,7 @@
     <t>Verhindern, dass Lebensmittel ablaufen und somit im Müll landen</t>
   </si>
   <si>
-    <t>Einzelhaushalte</t>
+    <t>Business Kunden</t>
   </si>
   <si>
     <t>So frisch wie möglich</t>
@@ -64,7 +67,7 @@
     <t>Hilfe für eine bessere Ernährung zu liefern</t>
   </si>
   <si>
-    <t>Ernährungsbewusste(Sportler, ...)</t>
+    <t>Ernährungsbewusste</t>
   </si>
   <si>
     <t>Übersicht über die Ernährung und eventuelle Gesundheitsempfehlung</t>
@@ -76,7 +79,7 @@
     <t>Kooperation mit Smart Device Herstellern zur Integration der App</t>
   </si>
   <si>
-    <t>Smart Device Hersteller(Partner)</t>
+    <t>-</t>
   </si>
   <si>
     <t>Am besten füllt der Kühlschrank sich von selbst</t>
@@ -85,19 +88,10 @@
     <t>Einscannen von Kassenzettel mit direkter Inventarliste</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Einzelhandel(Partner)</t>
-  </si>
-  <si>
     <t>Rezeptempfehlungen für vorhandenes Inventar</t>
   </si>
   <si>
-    <t>Restaurants</t>
-  </si>
-  <si>
-    <t>Konkurrenz</t>
+    <t>Konkurrenz*</t>
   </si>
   <si>
     <t>Umsatz</t>
@@ -161,16 +155,32 @@
   </si>
   <si>
     <t>Out of Milk</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Quelle: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://www.connect.de/ratgeber/vorrat-verwalten-einkaufsliste-apps-ios-android-3200639.html</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -184,6 +194,7 @@
     <font>
       <b/>
       <sz val="14.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -194,6 +205,10 @@
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="6">
@@ -308,39 +323,45 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="6" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="5" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="6" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,240 +585,253 @@
     <col customWidth="1" min="5" max="5" width="29.57"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" ht="38.25" customHeight="1">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3">
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5">
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="E8" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="E9" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
+    </row>
+    <row r="13">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="C14" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="E14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="10" t="s">
+    </row>
+    <row r="15">
+      <c r="B15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="C15" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="E15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="10" t="s">
+    </row>
+    <row r="16">
+      <c r="B16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="C16" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="10" t="s">
+      <c r="D16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="E16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="10" t="s">
+    </row>
+    <row r="17">
+      <c r="B17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="10" t="s">
+    </row>
+    <row r="18">
+      <c r="B18" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="C18" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B21"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>